<commit_message>
update a book successfully in NewBookWindow
</commit_message>
<xml_diff>
--- a/documents/Tasks.xlsx
+++ b/documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIU\1my studies\2-mpp\project\library-system\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A936D66-6B51-47F8-8A5C-48F02CAC8CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4163D95F-FCB6-4027-A63B-A9BA51753108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="2" xr2:uid="{08E91735-19BF-4484-930C-930DAB346417}"/>
+    <workbookView xWindow="4710" yWindow="2310" windowWidth="17280" windowHeight="9982" activeTab="1" xr2:uid="{08E91735-19BF-4484-930C-930DAB346417}"/>
   </bookViews>
   <sheets>
     <sheet name="Modeling" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>#</t>
   </si>
@@ -111,6 +111,28 @@
   </si>
   <si>
     <t>Add a new member</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>- CRUD a book
+- input validation</t>
+  </si>
+  <si>
+    <t>- CRUD a member
+- input validation</t>
+  </si>
+  <si>
+    <t>- CRUD a book copy
+- input validation</t>
+  </si>
+  <si>
+    <t>- login
+- show/hide corresponding menus</t>
   </si>
 </sst>
 </file>
@@ -705,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C76E1F9-5913-4950-8219-BBF36F439E12}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -714,7 +736,7 @@
     <col min="1" max="1" width="1.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
@@ -745,7 +767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -755,9 +777,11 @@
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -767,9 +791,11 @@
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -779,7 +805,9 @@
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
@@ -793,7 +821,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -803,14 +831,20 @@
       <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -900,7 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D0F7A0-BFB5-4F73-A7F2-F17368F4BAFE}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
submit work for checkout form - update availability successfully
</commit_message>
<xml_diff>
--- a/documents/Tasks.xlsx
+++ b/documents/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIU\1my studies\2-mpp\project\library-system\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4163D95F-FCB6-4027-A63B-A9BA51753108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A0E0B4-998C-4EB7-A8B9-DF92BD667E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4710" yWindow="2310" windowWidth="17280" windowHeight="9982" activeTab="1" xr2:uid="{08E91735-19BF-4484-930C-930DAB346417}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>#</t>
   </si>
@@ -133,6 +133,12 @@
   <si>
     <t>- login
 - show/hide corresponding menus</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>without authors</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -185,17 +191,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,10 +753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C76E1F9-5913-4950-8219-BBF36F439E12}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -737,9 +765,10 @@
     <col min="2" max="2" width="19.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.46484375" customWidth="1"/>
+    <col min="5" max="5" width="1.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -766,8 +795,11 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -775,13 +807,16 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -794,8 +829,11 @@
       <c r="D4" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -808,8 +846,14 @@
       <c r="D5" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -820,8 +864,11 @@
         <v>19</v>
       </c>
       <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E6" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -834,8 +881,11 @@
       <c r="D7" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -847,49 +897,49 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>

<commit_message>
update NewBookWindow to handle add a book with authors selection
</commit_message>
<xml_diff>
--- a/documents/Tasks.xlsx
+++ b/documents/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIU\1my studies\2-mpp\project\library-system\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A0E0B4-998C-4EB7-A8B9-DF92BD667E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01134FA6-CD5C-47D2-8BF9-50F4A15DE71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4710" yWindow="2310" windowWidth="17280" windowHeight="9982" activeTab="1" xr2:uid="{08E91735-19BF-4484-930C-930DAB346417}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>#</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>without authors</t>
   </si>
 </sst>
 </file>
@@ -222,8 +219,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,7 +753,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -829,9 +826,7 @@
       <c r="D4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
@@ -849,9 +844,7 @@
       <c r="E5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
@@ -881,9 +874,7 @@
       <c r="D7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="2">

</xml_diff>

<commit_message>
finalize the project with documents
</commit_message>
<xml_diff>
--- a/documents/Tasks.xlsx
+++ b/documents/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIU\1my studies\2-mpp\project\library-system\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F5DE1B-315E-4BD8-BC69-C1DE2B9E082C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C57AC0-A77F-491F-9806-22028CB61BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="2310" windowWidth="17280" windowHeight="9982" xr2:uid="{08E91735-19BF-4484-930C-930DAB346417}"/>
+    <workbookView xWindow="4710" yWindow="2310" windowWidth="17280" windowHeight="9982" activeTab="1" xr2:uid="{08E91735-19BF-4484-930C-930DAB346417}"/>
   </bookViews>
   <sheets>
     <sheet name="Modeling" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>#</t>
   </si>
@@ -125,17 +125,28 @@
 - input validation</t>
   </si>
   <si>
-    <t>- login
+    <t>x</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Performer</t>
+  </si>
+  <si>
+    <t>- one general class diagram
+- one for new member use case</t>
+  </si>
+  <si>
+    <t>STC conclusion</t>
+  </si>
+  <si>
+    <t>- login/logout
 - show/hide corresponding menus</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Assignee</t>
-  </si>
-  <si>
-    <t>Performer</t>
+    <t>- input validation
+- check availability of book</t>
   </si>
 </sst>
 </file>
@@ -557,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF3E5CE-F8AA-44F0-A715-3D7FBD129E37}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -567,7 +578,7 @@
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
@@ -578,10 +589,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -602,7 +613,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -615,7 +626,9 @@
       <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
@@ -627,7 +640,9 @@
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
@@ -642,7 +657,9 @@
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
@@ -657,7 +674,9 @@
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
@@ -780,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C76E1F9-5913-4950-8219-BBF36F439E12}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -802,10 +821,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -828,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -845,10 +864,10 @@
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -884,11 +903,11 @@
         <v>24</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -901,9 +920,11 @@
       <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="F6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -1038,7 +1059,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1058,10 +1079,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1086,8 +1107,12 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>